<commit_message>
Make all of the links actual hyperlinks in excel.
</commit_message>
<xml_diff>
--- a/bom/BOM.xlsx
+++ b/bom/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t xml:space="preserve">Item Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">LPMC1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lantern Power Monitor Case Lid</t>
   </si>
   <si>
@@ -61,142 +58,91 @@
     <t xml:space="preserve">LPMPCB1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/pcb</t>
-  </si>
-  <si>
     <t xml:space="preserve">Raspberry Pi 3 Model A+</t>
   </si>
   <si>
     <t xml:space="preserve">3A+</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.raspberrypi.org/products/raspberry-pi-3-model-a-plus/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jameco 12V AC/AC Adapter</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.jameco.com/z/ACU120100Z9121-Jameco-Reliapro-AC-to-AC-Wall-Adapter-Transformer-12-Volt-AC-1000mA-Black-Straight-3-5mm-Male-Plug_10428.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">16gb memory card</t>
   </si>
   <si>
     <t xml:space="preserve">P-SDU16GU185GW-GE</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.microcenter.com/product/486146/micro-center-16gb-microsdhc-class-10-flash-memory-card</t>
-  </si>
-  <si>
     <t xml:space="preserve">40-pin GPIO header</t>
   </si>
   <si>
     <t xml:space="preserve">C169819</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C169819_C169819.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">MCP3008</t>
   </si>
   <si>
     <t xml:space="preserve">MCP3008-I-P</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/microchip-technology/MCP3008-I-P/319422</t>
-  </si>
-  <si>
     <t xml:space="preserve">10uF 25V 4*5 Capacitor</t>
   </si>
   <si>
     <t xml:space="preserve">C43846</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-10uF-25V-4-5_C43846.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">22uF 25V 4*7 Capacitor</t>
   </si>
   <si>
     <t xml:space="preserve">C43840</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-22uF-25V-4-7_C43840.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">10KΩ Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">C385441</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS10K%CE%A9FT-BA1_C385441.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">12KΩ Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">C385449</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS12K%CE%A9FT-BA1_C385449.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">180KΩ Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">C385460</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS180K%CE%A9FT-BA1_C385460.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">33KΩ Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">C385498</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS33K%CE%A9FT-BA1_C385498.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">68KΩ Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">C385541</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS68K%CE%A9FT-BA1_C385541.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.5mm Headphone Jack</t>
   </si>
   <si>
     <t xml:space="preserve">PJ-3583-B</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Audio-Video-Connectors_XKB-Enterprise-PJ-3583-B_C397337.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">M2.5x10mm Cap Screw</t>
   </si>
   <si>
     <t xml:space="preserve">A15120300ux0225</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.amazon.com/gp/product/B01B1OD7IK</t>
-  </si>
-  <si>
     <t xml:space="preserve">M2.5x11mm Female x Female Standoff</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ebay.com/itm/50pcs-M2-5-Female-Hex-Screw-Brass-PCB-Standoffs-Hexagonal-Spacers/172746413434</t>
-  </si>
-  <si>
     <t xml:space="preserve">M2.5x12mm Female x Male Standoff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.ebay.com/itm/M2-5-2-5mm-Thread-6mm-Brass-Standoff-Spacer-Male-x-Female-20-50pcs-New/283432513974</t>
   </si>
   <si>
     <t xml:space="preserve">50 Amp Current Transformer</t>
@@ -232,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,6 +200,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,10 +278,10 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.88"/>
@@ -362,8 +310,9 @@
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
+      <c r="C2" s="0" t="str">
+        <f aca="false">HYPERLINK("https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case","https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case")</f>
+        <v>https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -371,13 +320,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
+      <c r="C3" s="0" t="str">
+        <f aca="false">HYPERLINK("https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case","https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case")</f>
+        <v>https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -385,13 +335,14 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
+      <c r="C4" s="0" t="str">
+        <f aca="false">HYPERLINK("https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case","https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case")</f>
+        <v>https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/case</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -399,13 +350,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>13</v>
+      <c r="C5" s="0" t="str">
+        <f aca="false">HYPERLINK("https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/pcb","https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/pcb")</f>
+        <v>https://github.com/MarkBryanMilligan/LanternPowerMonitor/tree/main/pcb</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -413,13 +365,14 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.raspberrypi.org/products/raspberry-pi-3-model-a-plus/","https://www.raspberrypi.org/products/raspberry-pi-3-model-a-plus/")</f>
+        <v>https://www.raspberrypi.org/products/raspberry-pi-3-model-a-plus/</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -427,13 +380,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>10428</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>18</v>
+      <c r="C7" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.jameco.com/z/ACU120100Z9121-Jameco-Reliapro-AC-to-AC-Wall-Adapter-Transformer-12-Volt-AC-1000mA-Black-Straight-3-5mm-Male-Plug_10428.html","https://www.jameco.com/z/ACU120100Z9121-Jameco-Reliapro-AC-to-AC-Wall-Adapter-Transformer-12-Volt-AC-1000mA-Black-Straight-3-5mm-Male-Plug_10428.html")</f>
+        <v>https://www.jameco.com/z/ACU120100Z9121-Jameco-Reliapro-AC-to-AC-Wall-Adapter-Transformer-12-Volt-AC-1000mA-Black-Straight-3-5mm-Male-Plug_10428.html</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -441,13 +395,14 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.microcenter.com/product/486146/micro-center-16gb-microsdhc-class-10-flash-memory-card","https://www.microcenter.com/product/486146/micro-center-16gb-microsdhc-class-10-flash-memory-card")</f>
+        <v>https://www.microcenter.com/product/486146/micro-center-16gb-microsdhc-class-10-flash-memory-card</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -455,13 +410,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C169819_C169819.html","https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C169819_C169819.html")</f>
+        <v>https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C169819_C169819.html</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -469,13 +425,14 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/MCP3008-I-P/319422","https://www.digikey.com/en/products/detail/microchip-technology/MCP3008-I-P/319422")</f>
+        <v>https://www.digikey.com/en/products/detail/microchip-technology/MCP3008-I-P/319422</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
@@ -483,13 +440,14 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-10uF-25V-4-5_C43846.html","https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-10uF-25V-4-5_C43846.html")</f>
+        <v>https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-10uF-25V-4-5_C43846.html</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -497,13 +455,14 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-22uF-25V-4-7_C43840.html","https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-22uF-25V-4-7_C43840.html")</f>
+        <v>https://lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-Leaded_CX-Dongguan-Chengxing-Elec-22uF-25V-4-7_C43840.html</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -511,13 +470,14 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS10K%CE%A9FT-BA1_C385441.html","https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS10K%CE%A9FT-BA1_C385441.html")</f>
+        <v>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS10K%CE%A9FT-BA1_C385441.html</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -525,13 +485,14 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS12K%CE%A9FT-BA1_C385449.html","https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS12K%CE%A9FT-BA1_C385449.html")</f>
+        <v>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS12K%CE%A9FT-BA1_C385449.html</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -539,13 +500,14 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS180K%CE%A9FT-BA1_C385460.html","https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS180K%CE%A9FT-BA1_C385460.html")</f>
+        <v>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS180K%CE%A9FT-BA1_C385460.html</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -553,13 +515,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS33K%CE%A9FT-BA1_C385498.html","https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS33K%CE%A9FT-BA1_C385498.html")</f>
+        <v>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS33K%CE%A9FT-BA1_C385498.html</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -567,13 +530,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS68K%CE%A9FT-BA1_C385541.html","https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS68K%CE%A9FT-BA1_C385541.html")</f>
+        <v>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TyoHM-RN1-2WS68K%CE%A9FT-BA1_C385541.html</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -581,13 +545,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="str">
+        <f aca="false">HYPERLINK("https://lcsc.com/product-detail/Audio-Video-Connectors_XKB-Enterprise-PJ-3583-B_C397337.html","https://lcsc.com/product-detail/Audio-Video-Connectors_XKB-Enterprise-PJ-3583-B_C397337.html")</f>
+        <v>https://lcsc.com/product-detail/Audio-Video-Connectors_XKB-Enterprise-PJ-3583-B_C397337.html</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>16</v>
@@ -595,13 +560,14 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="C19" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.amazon.com/gp/product/B01B1OD7IK","https://www.amazon.com/gp/product/B01B1OD7IK")</f>
+        <v>https://www.amazon.com/gp/product/B01B1OD7IK</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>8</v>
@@ -609,10 +575,11 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.ebay.com/itm/50pcs-M2-5-Female-Hex-Screw-Brass-PCB-Standoffs-Hexagonal-Spacers/172746413434","https://www.ebay.com/itm/50pcs-M2-5-Female-Hex-Screw-Brass-PCB-Standoffs-Hexagonal-Spacers/172746413434")</f>
+        <v>https://www.ebay.com/itm/50pcs-M2-5-Female-Hex-Screw-Brass-PCB-Standoffs-Hexagonal-Spacers/172746413434</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>4</v>
@@ -620,10 +587,11 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>58</v>
+        <v>40</v>
+      </c>
+      <c r="C21" s="0" t="str">
+        <f aca="false">HYPERLINK("https://www.ebay.com/itm/M2-5-2-5mm-Thread-6mm-Brass-Standoff-Spacer-Male-x-Female-20-50pcs-New/283432513974","https://www.ebay.com/itm/M2-5-2-5mm-Thread-6mm-Brass-Standoff-Spacer-Male-x-Female-20-50pcs-New/283432513974")</f>
+        <v>https://www.ebay.com/itm/M2-5-2-5mm-Thread-6mm-Brass-Standoff-Spacer-Male-x-Female-20-50pcs-New/283432513974</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>4</v>
@@ -631,36 +599,36 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update BOM for out of stock parts
</commit_message>
<xml_diff>
--- a/bom/BOM.xlsx
+++ b/bom/BOM.xlsx
@@ -124,13 +124,13 @@
     <t xml:space="preserve">68KΩ Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">C385541</t>
+    <t xml:space="preserve">C433508</t>
   </si>
   <si>
     <t xml:space="preserve">3.5mm Headphone Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">PJ-3583-B</t>
+    <t xml:space="preserve">C397337</t>
   </si>
   <si>
     <t xml:space="preserve">M2.5x10mm Cap Screw</t>
@@ -278,10 +278,10 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.88"/>
@@ -635,7 +635,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>